<commit_message>
Plein de truc la
</commit_message>
<xml_diff>
--- a/doc/C61_-_Sprint_1_-_Document_de_planification.xlsx
+++ b/doc/C61_-_Sprint_1_-_Document_de_planification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crage\Desktop\C61_SHOGI_RAG\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\Ecole\Session_Hiver_2025\C61_SHOGI_RAG\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0940DF3-7961-4954-ACE7-69AB6A83D9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4A3AEB-2D2A-4B09-96F8-6B9EE593F6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planification" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="205">
   <si>
     <t>Planification globale</t>
   </si>
@@ -632,6 +632,18 @@
   </si>
   <si>
     <t>reglage de bug lier au gameSaver</t>
+  </si>
+  <si>
+    <t>Reglage de bug lier au pièces</t>
+  </si>
+  <si>
+    <t>Reglage de bug, Minimax ne jouait plus</t>
+  </si>
+  <si>
+    <t>Ménage de code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retiré les commentaires non pertinent, tabulations et espaces ajusté </t>
   </si>
 </sst>
 </file>
@@ -706,20 +718,21 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -740,14 +753,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -846,13 +852,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1029,6 +1036,12 @@
     <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1041,49 +1054,49 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Excel Built-in Neutral" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Excel Built-in Neutral 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Neutre" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -3297,32 +3310,32 @@
     </row>
     <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="21"/>
-      <c r="B3" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="69" t="s">
+      <c r="B3" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70" t="s">
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="71" t="s">
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
     </row>
     <row r="4" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="21"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="3" t="s">
         <v>98</v>
       </c>
@@ -3484,7 +3497,7 @@
       <c r="E11" s="29">
         <v>1</v>
       </c>
-      <c r="F11" s="72" t="s">
+      <c r="F11" s="68" t="s">
         <v>103</v>
       </c>
       <c r="G11" s="28"/>
@@ -3507,7 +3520,7 @@
       <c r="E12" s="29">
         <v>1</v>
       </c>
-      <c r="F12" s="72"/>
+      <c r="F12" s="68"/>
       <c r="G12" s="28"/>
       <c r="H12" s="29"/>
       <c r="I12" s="30"/>
@@ -3528,7 +3541,7 @@
       <c r="E13" s="29">
         <v>1</v>
       </c>
-      <c r="F13" s="72"/>
+      <c r="F13" s="68"/>
       <c r="G13" s="28"/>
       <c r="H13" s="29"/>
       <c r="I13" s="30"/>
@@ -3549,7 +3562,7 @@
       <c r="E14" s="29">
         <v>1</v>
       </c>
-      <c r="F14" s="72"/>
+      <c r="F14" s="68"/>
       <c r="G14" s="28"/>
       <c r="H14" s="29"/>
       <c r="I14" s="30"/>
@@ -3570,7 +3583,7 @@
       <c r="E15" s="29">
         <v>1</v>
       </c>
-      <c r="F15" s="72"/>
+      <c r="F15" s="68"/>
       <c r="G15" s="28"/>
       <c r="H15" s="29"/>
       <c r="I15" s="30"/>
@@ -3591,7 +3604,7 @@
       <c r="E16" s="29">
         <v>1</v>
       </c>
-      <c r="F16" s="72"/>
+      <c r="F16" s="68"/>
       <c r="G16" s="28"/>
       <c r="H16" s="29"/>
       <c r="I16" s="30"/>
@@ -3612,7 +3625,7 @@
       <c r="E17" s="29">
         <v>1</v>
       </c>
-      <c r="F17" s="72"/>
+      <c r="F17" s="68"/>
       <c r="G17" s="28"/>
       <c r="H17" s="29"/>
       <c r="I17" s="30"/>
@@ -3995,7 +4008,7 @@
       <c r="K35" s="41">
         <v>1</v>
       </c>
-      <c r="L35" s="72" t="s">
+      <c r="L35" s="68" t="s">
         <v>127</v>
       </c>
     </row>
@@ -4018,7 +4031,7 @@
       <c r="K36" s="29">
         <v>1</v>
       </c>
-      <c r="L36" s="72"/>
+      <c r="L36" s="68"/>
     </row>
     <row r="37" spans="1:12" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="38" t="s">
@@ -4039,7 +4052,7 @@
       <c r="K37" s="29">
         <v>0.3</v>
       </c>
-      <c r="L37" s="72"/>
+      <c r="L37" s="68"/>
     </row>
     <row r="38" spans="1:12" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="38" t="s">
@@ -4347,7 +4360,7 @@
       <c r="K53" s="29">
         <v>1</v>
       </c>
-      <c r="L53" s="73" t="s">
+      <c r="L53" s="69" t="s">
         <v>137</v>
       </c>
     </row>
@@ -4366,7 +4379,7 @@
       <c r="I54" s="30"/>
       <c r="J54" s="28"/>
       <c r="K54" s="29"/>
-      <c r="L54" s="73"/>
+      <c r="L54" s="69"/>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="38" t="s">
@@ -4383,7 +4396,7 @@
       <c r="I55" s="30"/>
       <c r="J55" s="28"/>
       <c r="K55" s="29"/>
-      <c r="L55" s="73"/>
+      <c r="L55" s="69"/>
     </row>
     <row r="56" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="38" t="s">
@@ -4398,7 +4411,7 @@
       <c r="E56" s="29">
         <v>0.9</v>
       </c>
-      <c r="F56" s="72" t="s">
+      <c r="F56" s="68" t="s">
         <v>138</v>
       </c>
       <c r="G56" s="28"/>
@@ -4406,7 +4419,7 @@
       <c r="I56" s="30"/>
       <c r="J56" s="28"/>
       <c r="K56" s="29"/>
-      <c r="L56" s="73"/>
+      <c r="L56" s="69"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" s="38" t="s">
@@ -4421,7 +4434,7 @@
       <c r="E57" s="29">
         <v>0.9</v>
       </c>
-      <c r="F57" s="72"/>
+      <c r="F57" s="68"/>
       <c r="G57" s="28"/>
       <c r="H57" s="29"/>
       <c r="I57" s="30"/>
@@ -4442,7 +4455,7 @@
       <c r="E58" s="29">
         <v>0.9</v>
       </c>
-      <c r="F58" s="72"/>
+      <c r="F58" s="68"/>
       <c r="G58" s="28"/>
       <c r="H58" s="29"/>
       <c r="I58" s="30"/>
@@ -4463,7 +4476,7 @@
       <c r="E59" s="29">
         <v>0.9</v>
       </c>
-      <c r="F59" s="72"/>
+      <c r="F59" s="68"/>
       <c r="G59" s="28"/>
       <c r="H59" s="29"/>
       <c r="I59" s="30"/>
@@ -4484,7 +4497,7 @@
       <c r="E60" s="29">
         <v>0.9</v>
       </c>
-      <c r="F60" s="72"/>
+      <c r="F60" s="68"/>
       <c r="G60" s="28"/>
       <c r="H60" s="29"/>
       <c r="I60" s="30"/>
@@ -4505,7 +4518,7 @@
       <c r="E61" s="29">
         <v>0.9</v>
       </c>
-      <c r="F61" s="72"/>
+      <c r="F61" s="68"/>
       <c r="G61" s="28"/>
       <c r="H61" s="29"/>
       <c r="I61" s="30"/>
@@ -4526,7 +4539,7 @@
       <c r="E62" s="29">
         <v>0.9</v>
       </c>
-      <c r="F62" s="72"/>
+      <c r="F62" s="68"/>
       <c r="G62" s="28"/>
       <c r="H62" s="29"/>
       <c r="I62" s="30"/>
@@ -4547,7 +4560,7 @@
       <c r="E63" s="29">
         <v>0.9</v>
       </c>
-      <c r="F63" s="72"/>
+      <c r="F63" s="68"/>
       <c r="G63" s="28"/>
       <c r="H63" s="29"/>
       <c r="I63" s="30"/>
@@ -4568,7 +4581,7 @@
       <c r="E64" s="29">
         <v>0.9</v>
       </c>
-      <c r="F64" s="72"/>
+      <c r="F64" s="68"/>
       <c r="G64" s="28"/>
       <c r="H64" s="29"/>
       <c r="I64" s="30"/>
@@ -4589,7 +4602,7 @@
       <c r="E65" s="29">
         <v>0.9</v>
       </c>
-      <c r="F65" s="72"/>
+      <c r="F65" s="68"/>
       <c r="G65" s="28"/>
       <c r="H65" s="29"/>
       <c r="I65" s="30"/>
@@ -4617,7 +4630,7 @@
       <c r="H66" s="29">
         <v>1</v>
       </c>
-      <c r="I66" s="73" t="s">
+      <c r="I66" s="69" t="s">
         <v>139</v>
       </c>
       <c r="J66" s="28"/>
@@ -4632,7 +4645,7 @@
       <c r="F67" s="30"/>
       <c r="G67" s="28"/>
       <c r="H67" s="29"/>
-      <c r="I67" s="73"/>
+      <c r="I67" s="69"/>
       <c r="J67" s="28"/>
       <c r="K67" s="29"/>
       <c r="L67" s="30"/>
@@ -4743,16 +4756,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="J3:L3"/>
     <mergeCell ref="F11:F17"/>
     <mergeCell ref="L35:L37"/>
     <mergeCell ref="L53:L56"/>
     <mergeCell ref="F56:F65"/>
     <mergeCell ref="I66:I67"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="J3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4763,7 +4776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:L67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -4781,31 +4794,31 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="75" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="69" t="s">
+      <c r="B3" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70" t="s">
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="71" t="s">
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
     </row>
     <row r="4" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="75"/>
-      <c r="C4" s="69"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="3" t="s">
         <v>91</v>
       </c>
@@ -5094,7 +5107,7 @@
       <c r="E18" s="67">
         <v>0.8</v>
       </c>
-      <c r="F18" s="73" t="s">
+      <c r="F18" s="69" t="s">
         <v>198</v>
       </c>
       <c r="G18" s="28"/>
@@ -5113,7 +5126,7 @@
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="73"/>
+      <c r="F19" s="69"/>
       <c r="G19" s="28" t="s">
         <v>104</v>
       </c>
@@ -5134,7 +5147,7 @@
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
-      <c r="F20" s="73"/>
+      <c r="F20" s="69"/>
       <c r="G20" s="28" t="s">
         <v>39</v>
       </c>
@@ -5318,7 +5331,7 @@
       <c r="H29" s="67">
         <v>0.7</v>
       </c>
-      <c r="I29" s="73" t="s">
+      <c r="I29" s="69" t="s">
         <v>197</v>
       </c>
       <c r="J29" s="28"/>
@@ -5333,7 +5346,7 @@
       <c r="F30" s="27"/>
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
-      <c r="I30" s="73"/>
+      <c r="I30" s="69"/>
       <c r="J30" s="28"/>
       <c r="K30" s="28"/>
       <c r="L30" s="27"/>
@@ -5351,7 +5364,7 @@
       <c r="E31" s="67">
         <v>0.75</v>
       </c>
-      <c r="F31" s="73" t="s">
+      <c r="F31" s="69" t="s">
         <v>195</v>
       </c>
       <c r="G31" s="28"/>
@@ -5378,7 +5391,7 @@
       <c r="E32" s="67">
         <v>0.75</v>
       </c>
-      <c r="F32" s="73"/>
+      <c r="F32" s="69"/>
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
       <c r="I32" s="27"/>
@@ -5514,7 +5527,7 @@
       <c r="H39" s="67">
         <v>1</v>
       </c>
-      <c r="I39" s="74"/>
+      <c r="I39" s="75"/>
       <c r="J39" s="28"/>
       <c r="K39" s="28"/>
       <c r="L39" s="27"/>
@@ -5535,7 +5548,7 @@
       <c r="H40" s="67">
         <v>1</v>
       </c>
-      <c r="I40" s="74"/>
+      <c r="I40" s="75"/>
       <c r="J40" s="28"/>
       <c r="K40" s="28"/>
       <c r="L40" s="27"/>
@@ -5605,7 +5618,7 @@
       <c r="H44" s="67">
         <v>1</v>
       </c>
-      <c r="I44" s="72" t="s">
+      <c r="I44" s="68" t="s">
         <v>193</v>
       </c>
       <c r="J44" s="28"/>
@@ -5628,7 +5641,7 @@
       <c r="H45" s="67">
         <v>1</v>
       </c>
-      <c r="I45" s="72"/>
+      <c r="I45" s="68"/>
       <c r="J45" s="28"/>
       <c r="K45" s="28"/>
       <c r="L45" s="27"/>
@@ -5649,7 +5662,7 @@
       <c r="H46" s="67">
         <v>1</v>
       </c>
-      <c r="I46" s="72"/>
+      <c r="I46" s="68"/>
       <c r="J46" s="28"/>
       <c r="K46" s="28"/>
       <c r="L46" s="27"/>
@@ -5670,7 +5683,7 @@
       <c r="H47" s="67">
         <v>1</v>
       </c>
-      <c r="I47" s="72"/>
+      <c r="I47" s="68"/>
       <c r="J47" s="28"/>
       <c r="K47" s="28"/>
       <c r="L47" s="27"/>
@@ -5691,7 +5704,7 @@
       <c r="H48" s="67">
         <v>1</v>
       </c>
-      <c r="I48" s="72"/>
+      <c r="I48" s="68"/>
       <c r="J48" s="28"/>
       <c r="K48" s="28"/>
       <c r="L48" s="27"/>
@@ -6003,16 +6016,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I44:I48"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="F18:F20"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="J3:L3"/>
-    <mergeCell ref="I44:I48"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="F18:F20"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -6022,10 +6035,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B1:O41"/>
+  <dimension ref="B1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6033,15 +6046,7 @@
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
     <col min="2" max="2" width="47.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" customWidth="1"/>
-    <col min="15" max="15" width="20.28515625" customWidth="1"/>
+    <col min="4" max="15" width="19" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="46.5" x14ac:dyDescent="0.7">
@@ -6052,26 +6057,28 @@
     <row r="3" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="16"/>
       <c r="C3" s="17"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17" t="s">
+      <c r="E3" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="17" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="N3" s="17"/>
-      <c r="O3" s="18"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="2"/>
     </row>
     <row r="4" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="16" t="s">
@@ -6083,494 +6090,722 @@
       <c r="D4" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="66" t="s">
-        <v>89</v>
-      </c>
+      <c r="E4" s="71"/>
       <c r="F4" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="O4" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="2:15" s="22" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="86" t="s">
+    <row r="5" spans="2:15" s="22" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="77" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="79">
-        <v>1</v>
-      </c>
-      <c r="F5" s="80"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="80"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="80"/>
-    </row>
-    <row r="6" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="82" t="s">
+      <c r="E5" s="78">
+        <v>1</v>
+      </c>
+      <c r="F5" s="76"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="76"/>
+    </row>
+    <row r="6" spans="2:15" s="22" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="83"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="76"/>
+    </row>
+    <row r="7" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="82" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="83"/>
-      <c r="D6" s="84" t="s">
+      <c r="C7" s="79"/>
+      <c r="D7" s="80" t="s">
         <v>160</v>
       </c>
-      <c r="E6" s="79">
+      <c r="E7" s="78">
         <v>0.33</v>
       </c>
-      <c r="F6" s="85"/>
-      <c r="G6" s="84" t="s">
+      <c r="F7" s="81"/>
+      <c r="G7" s="80" t="s">
         <v>160</v>
       </c>
-      <c r="H6" s="79">
+      <c r="H7" s="78">
         <v>0.66</v>
       </c>
-      <c r="I6" s="85"/>
-      <c r="J6" s="84" t="s">
+      <c r="I7" s="81"/>
+      <c r="J7" s="80" t="s">
         <v>160</v>
       </c>
-      <c r="K6" s="79">
-        <v>1</v>
-      </c>
-      <c r="L6" s="85"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="79"/>
-      <c r="O6" s="85"/>
-    </row>
-    <row r="7" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="82" t="s">
+      <c r="K7" s="78">
+        <v>1</v>
+      </c>
+      <c r="L7" s="81"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="78"/>
+      <c r="O7" s="81"/>
+    </row>
+    <row r="8" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="82" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="83"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="84" t="s">
+      <c r="C8" s="79"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="80" t="s">
         <v>116</v>
       </c>
-      <c r="N7" s="79">
-        <v>1</v>
-      </c>
-      <c r="O7" s="85"/>
-    </row>
-    <row r="8" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="21"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="21"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="21"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="21"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="21"/>
-    </row>
-    <row r="9" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="21"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="21"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="21"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="21"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="21"/>
-    </row>
-    <row r="10" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="21"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="21"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="21"/>
-      <c r="K10" s="76"/>
-      <c r="L10" s="21"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="21"/>
-    </row>
-    <row r="11" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="21"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="21"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="21"/>
-      <c r="K11" s="76"/>
-      <c r="L11" s="21"/>
-      <c r="N11" s="76"/>
-      <c r="O11" s="21"/>
-    </row>
-    <row r="12" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="21"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="21"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="21"/>
-      <c r="K12" s="76"/>
-      <c r="L12" s="21"/>
-      <c r="N12" s="76"/>
-      <c r="O12" s="21"/>
-    </row>
-    <row r="13" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="21"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="21"/>
-      <c r="H13" s="76"/>
-      <c r="I13" s="21"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="21"/>
-      <c r="N13" s="76"/>
-      <c r="O13" s="21"/>
-    </row>
-    <row r="14" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-      <c r="C14" s="21"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="21"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="21"/>
-      <c r="K14" s="76"/>
-      <c r="L14" s="21"/>
-      <c r="N14" s="76"/>
-      <c r="O14" s="21"/>
-    </row>
-    <row r="15" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="21"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="21"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="21"/>
-      <c r="K15" s="76"/>
-      <c r="L15" s="21"/>
-      <c r="N15" s="76"/>
-      <c r="O15" s="21"/>
-    </row>
-    <row r="16" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
-      <c r="C16" s="21"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="21"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="21"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="21"/>
-      <c r="N16" s="76"/>
-      <c r="O16" s="21"/>
-    </row>
-    <row r="17" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="21"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="21"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="21"/>
-      <c r="K17" s="76"/>
-      <c r="L17" s="21"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="21"/>
-    </row>
-    <row r="18" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="21"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="21"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="21"/>
-      <c r="K18" s="76"/>
-      <c r="L18" s="21"/>
-      <c r="N18" s="76"/>
-      <c r="O18" s="21"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="9"/>
-      <c r="C19" s="21"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="21"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="21"/>
-      <c r="K19" s="76"/>
-      <c r="L19" s="21"/>
-      <c r="N19" s="76"/>
-      <c r="O19" s="21"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="21"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="21"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="21"/>
-      <c r="K20" s="76"/>
-      <c r="L20" s="21"/>
-      <c r="N20" s="76"/>
-      <c r="O20" s="21"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="21"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="21"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="21"/>
-      <c r="K21" s="76"/>
-      <c r="L21" s="21"/>
-      <c r="N21" s="76"/>
-      <c r="O21" s="21"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
-      <c r="C22" s="21"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="21"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="21"/>
-      <c r="K22" s="76"/>
-      <c r="L22" s="21"/>
-      <c r="N22" s="76"/>
-      <c r="O22" s="21"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="21"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="21"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="21"/>
-      <c r="K23" s="76"/>
-      <c r="L23" s="21"/>
-      <c r="N23" s="76"/>
-      <c r="O23" s="21"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="C24" s="21"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="21"/>
-      <c r="H24" s="76"/>
-      <c r="I24" s="21"/>
-      <c r="K24" s="76"/>
-      <c r="L24" s="21"/>
-      <c r="N24" s="76"/>
-      <c r="O24" s="21"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="21"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="21"/>
-      <c r="H25" s="76"/>
-      <c r="I25" s="21"/>
-      <c r="K25" s="76"/>
-      <c r="L25" s="21"/>
-      <c r="N25" s="76"/>
-      <c r="O25" s="21"/>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="21"/>
-      <c r="E26" s="76"/>
-      <c r="F26" s="21"/>
-      <c r="H26" s="76"/>
-      <c r="I26" s="21"/>
-      <c r="K26" s="76"/>
-      <c r="L26" s="21"/>
-      <c r="N26" s="76"/>
-      <c r="O26" s="21"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="21"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="21"/>
-      <c r="H27" s="76"/>
-      <c r="I27" s="21"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="21"/>
-      <c r="N27" s="76"/>
-      <c r="O27" s="21"/>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
-      <c r="C28" s="21"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="21"/>
-      <c r="H28" s="76"/>
-      <c r="I28" s="21"/>
-      <c r="K28" s="76"/>
-      <c r="L28" s="21"/>
-      <c r="N28" s="76"/>
-      <c r="O28" s="21"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="9"/>
-      <c r="C29" s="21"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="21"/>
-      <c r="H29" s="76"/>
-      <c r="I29" s="21"/>
-      <c r="K29" s="76"/>
-      <c r="L29" s="21"/>
-      <c r="N29" s="76"/>
-      <c r="O29" s="21"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
-      <c r="C30" s="21"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="21"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="21"/>
-      <c r="K30" s="76"/>
-      <c r="L30" s="21"/>
-      <c r="N30" s="76"/>
-      <c r="O30" s="21"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="C31" s="21"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="21"/>
-      <c r="H31" s="76"/>
-      <c r="I31" s="21"/>
-      <c r="K31" s="76"/>
-      <c r="L31" s="21"/>
-      <c r="N31" s="76"/>
-      <c r="O31" s="21"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="9"/>
-      <c r="C32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="H32" s="76"/>
-      <c r="I32" s="21"/>
-      <c r="K32" s="76"/>
-      <c r="L32" s="21"/>
-      <c r="N32" s="76"/>
-      <c r="O32" s="21"/>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-      <c r="C33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="H33" s="76"/>
-      <c r="I33" s="21"/>
-      <c r="K33" s="76"/>
-      <c r="L33" s="21"/>
-      <c r="N33" s="76"/>
-      <c r="O33" s="21"/>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
-      <c r="C34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="21"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="21"/>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="9"/>
-      <c r="C35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="N35" s="76"/>
-      <c r="O35" s="21"/>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="9"/>
-      <c r="C36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="O36" s="21"/>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="9"/>
-      <c r="C37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="O37" s="21"/>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-      <c r="C38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="L38" s="21"/>
-      <c r="O38" s="21"/>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="9"/>
-      <c r="C39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="L39" s="21"/>
-      <c r="O39" s="21"/>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
-      <c r="C40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="L40" s="21"/>
-      <c r="O40" s="21"/>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="9"/>
-      <c r="C41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="O41" s="21"/>
+      <c r="N8" s="78">
+        <v>1</v>
+      </c>
+      <c r="O8" s="81"/>
+    </row>
+    <row r="9" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="82"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="81"/>
+    </row>
+    <row r="10" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="82" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="84" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="85" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="86">
+        <v>1</v>
+      </c>
+      <c r="F10" s="84"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="84"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="87" t="s">
+        <v>204</v>
+      </c>
+      <c r="M10" s="85"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="84"/>
+    </row>
+    <row r="11" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="82" t="s">
+        <v>202</v>
+      </c>
+      <c r="C11" s="84" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="85"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="85" t="s">
+        <v>161</v>
+      </c>
+      <c r="H11" s="86">
+        <v>1</v>
+      </c>
+      <c r="I11" s="84"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="85"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="84"/>
+    </row>
+    <row r="12" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="82" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="84" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="85"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="85" t="s">
+        <v>161</v>
+      </c>
+      <c r="K12" s="86">
+        <v>1</v>
+      </c>
+      <c r="L12" s="87"/>
+      <c r="M12" s="85"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="84"/>
+    </row>
+    <row r="13" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="82"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="87"/>
+      <c r="M13" s="85"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="84"/>
+    </row>
+    <row r="14" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="82"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="84"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="84"/>
+      <c r="M14" s="85"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="84"/>
+    </row>
+    <row r="15" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="82"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="84"/>
+      <c r="M15" s="85"/>
+      <c r="N15" s="86"/>
+      <c r="O15" s="84"/>
+    </row>
+    <row r="16" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="82"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="85"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="84"/>
+      <c r="M16" s="85"/>
+      <c r="N16" s="86"/>
+      <c r="O16" s="84"/>
+    </row>
+    <row r="17" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="82"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="84"/>
+      <c r="J17" s="85"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="84"/>
+      <c r="M17" s="85"/>
+      <c r="N17" s="86"/>
+      <c r="O17" s="84"/>
+    </row>
+    <row r="18" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="82"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="84"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="84"/>
+      <c r="M18" s="85"/>
+      <c r="N18" s="86"/>
+      <c r="O18" s="84"/>
+    </row>
+    <row r="19" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="82"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="86"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="84"/>
+      <c r="M19" s="85"/>
+      <c r="N19" s="86"/>
+      <c r="O19" s="84"/>
+    </row>
+    <row r="20" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="82"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="84"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="86"/>
+      <c r="L20" s="84"/>
+      <c r="M20" s="85"/>
+      <c r="N20" s="86"/>
+      <c r="O20" s="84"/>
+    </row>
+    <row r="21" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="82"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="86"/>
+      <c r="I21" s="84"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="86"/>
+      <c r="L21" s="84"/>
+      <c r="M21" s="85"/>
+      <c r="N21" s="86"/>
+      <c r="O21" s="84"/>
+    </row>
+    <row r="22" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="82"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="86"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="85"/>
+      <c r="N22" s="86"/>
+      <c r="O22" s="84"/>
+    </row>
+    <row r="23" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="82"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="85"/>
+      <c r="N23" s="86"/>
+      <c r="O23" s="84"/>
+    </row>
+    <row r="24" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="82"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="84"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="86"/>
+      <c r="L24" s="84"/>
+      <c r="M24" s="85"/>
+      <c r="N24" s="86"/>
+      <c r="O24" s="84"/>
+    </row>
+    <row r="25" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="82"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="86"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="86"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="85"/>
+      <c r="N25" s="86"/>
+      <c r="O25" s="84"/>
+    </row>
+    <row r="26" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="82"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="84"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="86"/>
+      <c r="I26" s="84"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="86"/>
+      <c r="L26" s="84"/>
+      <c r="M26" s="85"/>
+      <c r="N26" s="86"/>
+      <c r="O26" s="84"/>
+    </row>
+    <row r="27" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="82"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="85"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="86"/>
+      <c r="I27" s="84"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="86"/>
+      <c r="L27" s="84"/>
+      <c r="M27" s="85"/>
+      <c r="N27" s="86"/>
+      <c r="O27" s="84"/>
+    </row>
+    <row r="28" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="82"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="85"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="84"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="84"/>
+      <c r="M28" s="85"/>
+      <c r="N28" s="86"/>
+      <c r="O28" s="84"/>
+    </row>
+    <row r="29" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="82"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="85"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="84"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="86"/>
+      <c r="I29" s="84"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="84"/>
+      <c r="M29" s="85"/>
+      <c r="N29" s="86"/>
+      <c r="O29" s="84"/>
+    </row>
+    <row r="30" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="82"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="85"/>
+      <c r="H30" s="86"/>
+      <c r="I30" s="84"/>
+      <c r="J30" s="85"/>
+      <c r="K30" s="86"/>
+      <c r="L30" s="84"/>
+      <c r="M30" s="85"/>
+      <c r="N30" s="86"/>
+      <c r="O30" s="84"/>
+    </row>
+    <row r="31" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="82"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="85"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="84"/>
+      <c r="G31" s="85"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="84"/>
+      <c r="J31" s="85"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="84"/>
+      <c r="M31" s="85"/>
+      <c r="N31" s="86"/>
+      <c r="O31" s="84"/>
+    </row>
+    <row r="32" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="82"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="85"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="85"/>
+      <c r="H32" s="86"/>
+      <c r="I32" s="84"/>
+      <c r="J32" s="85"/>
+      <c r="K32" s="86"/>
+      <c r="L32" s="84"/>
+      <c r="M32" s="85"/>
+      <c r="N32" s="86"/>
+      <c r="O32" s="84"/>
+    </row>
+    <row r="33" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="82"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="86"/>
+      <c r="F33" s="84"/>
+      <c r="G33" s="85"/>
+      <c r="H33" s="86"/>
+      <c r="I33" s="84"/>
+      <c r="J33" s="85"/>
+      <c r="K33" s="86"/>
+      <c r="L33" s="84"/>
+      <c r="M33" s="85"/>
+      <c r="N33" s="86"/>
+      <c r="O33" s="84"/>
+    </row>
+    <row r="34" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="82"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="85"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="86"/>
+      <c r="I34" s="84"/>
+      <c r="J34" s="85"/>
+      <c r="K34" s="86"/>
+      <c r="L34" s="84"/>
+      <c r="M34" s="85"/>
+      <c r="N34" s="86"/>
+      <c r="O34" s="84"/>
+    </row>
+    <row r="35" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="82"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="85"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="84"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="86"/>
+      <c r="I35" s="84"/>
+      <c r="J35" s="85"/>
+      <c r="K35" s="86"/>
+      <c r="L35" s="84"/>
+      <c r="M35" s="85"/>
+      <c r="N35" s="86"/>
+      <c r="O35" s="84"/>
+    </row>
+    <row r="36" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="82"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="84"/>
+      <c r="G36" s="85"/>
+      <c r="H36" s="85"/>
+      <c r="I36" s="84"/>
+      <c r="J36" s="85"/>
+      <c r="K36" s="86"/>
+      <c r="L36" s="84"/>
+      <c r="M36" s="85"/>
+      <c r="N36" s="86"/>
+      <c r="O36" s="84"/>
+    </row>
+    <row r="37" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="82"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="85"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="84"/>
+      <c r="J37" s="85"/>
+      <c r="K37" s="85"/>
+      <c r="L37" s="84"/>
+      <c r="M37" s="85"/>
+      <c r="N37" s="86"/>
+      <c r="O37" s="84"/>
+    </row>
+    <row r="38" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="82"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="85"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="84"/>
+      <c r="G38" s="85"/>
+      <c r="H38" s="85"/>
+      <c r="I38" s="84"/>
+      <c r="J38" s="85"/>
+      <c r="K38" s="85"/>
+      <c r="L38" s="84"/>
+      <c r="M38" s="85"/>
+      <c r="N38" s="85"/>
+      <c r="O38" s="84"/>
+    </row>
+    <row r="39" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="82"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="85"/>
+      <c r="E39" s="85"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="85"/>
+      <c r="I39" s="84"/>
+      <c r="J39" s="85"/>
+      <c r="K39" s="85"/>
+      <c r="L39" s="84"/>
+      <c r="M39" s="85"/>
+      <c r="N39" s="85"/>
+      <c r="O39" s="84"/>
+    </row>
+    <row r="40" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="82"/>
+      <c r="C40" s="79"/>
+      <c r="D40" s="85"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="85"/>
+      <c r="H40" s="85"/>
+      <c r="I40" s="84"/>
+      <c r="J40" s="85"/>
+      <c r="K40" s="85"/>
+      <c r="L40" s="84"/>
+      <c r="M40" s="85"/>
+      <c r="N40" s="85"/>
+      <c r="O40" s="84"/>
+    </row>
+    <row r="41" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="82"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="85"/>
+      <c r="E41" s="85"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="85"/>
+      <c r="H41" s="85"/>
+      <c r="I41" s="84"/>
+      <c r="J41" s="85"/>
+      <c r="K41" s="85"/>
+      <c r="L41" s="84"/>
+      <c r="M41" s="85"/>
+      <c r="N41" s="85"/>
+      <c r="O41" s="84"/>
+    </row>
+    <row r="42" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="82"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="85"/>
+      <c r="E42" s="85"/>
+      <c r="F42" s="84"/>
+      <c r="G42" s="85"/>
+      <c r="H42" s="85"/>
+      <c r="I42" s="84"/>
+      <c r="J42" s="85"/>
+      <c r="K42" s="85"/>
+      <c r="L42" s="84"/>
+      <c r="M42" s="85"/>
+      <c r="N42" s="85"/>
+      <c r="O42" s="84"/>
+    </row>
+    <row r="43" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="82"/>
+      <c r="C43" s="79"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="85"/>
+      <c r="F43" s="84"/>
+      <c r="G43" s="85"/>
+      <c r="H43" s="85"/>
+      <c r="I43" s="84"/>
+      <c r="J43" s="85"/>
+      <c r="K43" s="85"/>
+      <c r="L43" s="84"/>
+      <c r="M43" s="85"/>
+      <c r="N43" s="85"/>
+      <c r="O43" s="84"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="L10:L13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>